<commit_message>
Product mix 5 test cases, Data tables 15 Test Cases
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/4787-SUBMITSA01JAN2015(MINACTPRD-30DAYS&LCKINPRD-15DAYS)-APRACT01JAN2015.xlsx
+++ b/Mifos Automation Excels/Client/4787-SUBMITSA01JAN2015(MINACTPRD-30DAYS&LCKINPRD-15DAYS)-APRACT01JAN2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="NewShareInput" sheetId="1" r:id="rId1"/>
@@ -255,11 +255,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,10 +700,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -734,7 +734,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,10 +744,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -771,13 +771,11 @@
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4">
-        <v>86</v>
-      </c>
+      <c r="B5" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -856,7 +854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
@@ -878,7 +876,7 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>41</v>
       </c>
     </row>
@@ -934,7 +932,7 @@
       <c r="A9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>